<commit_message>
more changes to the code
</commit_message>
<xml_diff>
--- a/Projects/PEPSICOUK/Tests/Data/external_targets.xlsx
+++ b/Projects/PEPSICOUK/Tests/Data/external_targets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="external_targets" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="58">
   <si>
     <t xml:space="preserve">pk</t>
   </si>
@@ -161,6 +161,39 @@
   </si>
   <si>
     <t xml:space="preserve">{"KPI Parent": "Placement by shelf numbers", "Shelves From Bottom To Include (data)": "1,2"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"Group Name": "Pringles_FTT_Tubes"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"Target": 90, "Value 1": 189, "Value 2": "Fun times together Tubes", "Value 3": "", "Parameter 1": "brand_fk", "Parameter 2": "PDH Format", "Parameter 3": ""}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-04-01 00:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-04-03 09:38:27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Positioning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"Group Name": "Hula Hoops_LMP_Snacks"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"Target": 90, "Value 1": 138, "Value 2": "LMP Snacks", "Value 3": "", "Parameter 1": "brand_fk", "Parameter 2": "PDH Format", "Parameter 3": ""}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"Group Name": "DORITOS GROUP"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"Target": 0, "Value 1": 136, "Value 2": "", "Value 3": "", "Parameter 1": "brand_fk", "Parameter 2": "", "Parameter 3": ""}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"Group Name": "Walkers Crisps_Small MP PC"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"Target": 0, "Value 1": 199, "Value 2": 7, "Value 3": "SMP PC", "Parameter 1": "brand_fk", "Parameter 2": "sub_category_fk", "Parameter 3": "PDH Sub-segment"}</t>
   </si>
 </sst>
 </file>
@@ -262,21 +295,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="113.795918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="218.821428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="112.581632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="216.525510204082"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="17.4132653061224"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1118,6 +1150,122 @@
       </c>
       <c r="I29" s="0" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>319</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I30" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>319</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I31" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>316</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I32" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>316</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I33" s="0" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>